<commit_message>
Added new gerbers for the fabrication outputs for version 1.0
- Generated new fabrication outputs for the v1.0
- Corrected the resistor value for the reset pull up resistor (from 1k to 10k)
</commit_message>
<xml_diff>
--- a/Miniscope-v4-Wire-Free-KiCad/KiCad/Miniscope-v4-Wire-Free/Miniscope-v4-Wire-Free-BOM.xlsx
+++ b/Miniscope-v4-Wire-Free-KiCad/KiCad/Miniscope-v4-Wire-Free/Miniscope-v4-Wire-Free-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsang\Documents\Miniscope-v4-Wire-Free\Miniscope-v4-Wire-Free-KiCad\KiCad\Miniscope-v4-Wire-Free\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Federico\Documents\GitHub\Miniscope-v4-Wire-Free\Miniscope-v4-Wire-Free-KiCad\KiCad\Miniscope-v4-Wire-Free\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39B478B8-912D-4353-A55E-E3753DEA8877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A63B07E-4861-496C-A838-0E074F00BD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2190" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="-38520" yWindow="-5505" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Miniscope-v4-Wire-Free" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="189">
   <si>
     <t>Item</t>
   </si>
@@ -581,12 +581,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>ERJ-1GNF1002C</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/20W 0201</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1314,9 +1320,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1354,7 +1360,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1460,7 +1466,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1602,32 +1608,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="3" max="3" width="56.109375" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -1673,7 +1679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1719,7 +1725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1788,7 +1794,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1811,7 +1817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1834,7 +1840,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1857,7 +1863,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>475710001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1926,7 +1932,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1972,7 +1978,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1995,7 +2001,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2018,7 +2024,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2041,7 +2047,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2179,7 +2185,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -2225,7 +2231,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -2271,7 +2277,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -2294,7 +2300,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -2340,7 +2346,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -2363,7 +2369,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -2377,16 +2383,16 @@
         <v>134</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>113</v>
+        <v>188</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -2455,7 +2461,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -2478,7 +2484,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -2501,7 +2507,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -2593,7 +2599,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -2616,7 +2622,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>186</v>
       </c>

</xml_diff>